<commit_message>
Some more progress made
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ilja/Code/School/IoT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C296B405-32BA-CE4C-8F5C-EEE1073F9B38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4F9DED3-AFA1-2843-9A1B-5EAE5DD9B8A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{9D83B715-5ABF-CE44-818A-C1C3B282D9B7}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
   <si>
     <t>Blinky-blinky</t>
   </si>
@@ -78,9 +78,6 @@
     <t>Interrupt version of arduino lightswitch</t>
   </si>
   <si>
-    <t>I did my part</t>
-  </si>
-  <si>
     <t>Waiting to be discussed</t>
   </si>
   <si>
@@ -111,28 +108,46 @@
     <t>Visible light communications</t>
   </si>
   <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>T</t>
-  </si>
-  <si>
-    <t>K</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>L</t>
-  </si>
-  <si>
-    <t>P</t>
-  </si>
-  <si>
-    <t>code is ready, still need to measure voltage and amperage</t>
+    <t>#6</t>
+  </si>
+  <si>
+    <t>GIT</t>
+  </si>
+  <si>
+    <t>#5</t>
+  </si>
+  <si>
+    <t>#7</t>
+  </si>
+  <si>
+    <t>#8</t>
+  </si>
+  <si>
+    <t>#9</t>
+  </si>
+  <si>
+    <t>#10</t>
+  </si>
+  <si>
+    <t>#11</t>
+  </si>
+  <si>
+    <t>#12</t>
+  </si>
+  <si>
+    <t>#13</t>
+  </si>
+  <si>
+    <t>#14</t>
+  </si>
+  <si>
+    <t>I did my part, waiting for teacher to update rate</t>
+  </si>
+  <si>
+    <t>code is ready, consumption is measured</t>
+  </si>
+  <si>
+    <t>Date</t>
   </si>
 </sst>
 </file>
@@ -201,7 +216,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -516,19 +531,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B38C87C1-8F3E-6140-BC8A-D88B7B135530}">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="56" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" customWidth="1"/>
+    <col min="6" max="6" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="50.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1" s="1"/>
       <c r="C1" s="1" t="str">
         <f>_xlfn.CONCAT("Current ", SUM(C2:C99))</f>
@@ -538,8 +554,18 @@
         <f>_xlfn.CONCAT("Max ", SUM(D2:D99))</f>
         <v>Max 116</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E1" s="1" t="str">
+        <f>_xlfn.CONCAT("Coded ", SUM(E2:E99))</f>
+        <v>Coded 60</v>
+      </c>
+      <c r="F1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
@@ -549,8 +575,14 @@
       <c r="D2" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E2" s="2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
@@ -560,8 +592,14 @@
       <c r="D3" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E3" s="2">
+        <v>10</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -574,8 +612,14 @@
       <c r="D4" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E4" s="2">
+        <v>2</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2</v>
       </c>
@@ -588,8 +632,14 @@
       <c r="D5" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E5" s="2">
+        <v>2</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>3</v>
       </c>
@@ -602,8 +652,14 @@
       <c r="D6" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E6" s="2">
+        <v>3</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>4</v>
       </c>
@@ -616,8 +672,14 @@
       <c r="D7" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E7" s="2">
+        <v>3</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>5</v>
       </c>
@@ -630,8 +692,14 @@
       <c r="D8" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E8" s="2">
+        <v>3</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>6</v>
       </c>
@@ -644,8 +712,14 @@
       <c r="D9" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E9" s="2">
+        <v>3</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>7</v>
       </c>
@@ -658,8 +732,14 @@
       <c r="D10" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E10" s="2">
+        <v>5</v>
+      </c>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>8</v>
       </c>
@@ -672,8 +752,14 @@
       <c r="D11" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E11" s="2">
+        <v>4</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>9</v>
       </c>
@@ -686,11 +772,16 @@
       <c r="D12" s="3">
         <v>10</v>
       </c>
-      <c r="E12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E12" s="3">
+        <v>10</v>
+      </c>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>10</v>
       </c>
@@ -701,11 +792,16 @@
       <c r="D13" s="4">
         <v>4</v>
       </c>
-      <c r="E13" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E13" s="4">
+        <v>4</v>
+      </c>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>11</v>
       </c>
@@ -716,11 +812,16 @@
       <c r="D14" s="4">
         <v>4</v>
       </c>
-      <c r="E14" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E14" s="4">
+        <v>4</v>
+      </c>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>12</v>
       </c>
@@ -731,164 +832,177 @@
       <c r="D15" s="4">
         <v>3</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="4">
+        <v>3</v>
+      </c>
+      <c r="F15" s="6">
         <v>44494</v>
       </c>
-      <c r="F15" t="s">
-        <v>25</v>
-      </c>
-      <c r="G15" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D16">
         <v>3</v>
       </c>
-      <c r="E16" s="6">
+      <c r="F16" s="5">
         <v>44495</v>
       </c>
-      <c r="F16" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D17">
         <v>4</v>
       </c>
-      <c r="E17" s="6">
+      <c r="F17" s="5">
         <v>44496</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D18">
         <v>4</v>
       </c>
-      <c r="E18" s="6">
+      <c r="F18" s="5">
         <v>44497</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>16</v>
       </c>
-      <c r="B19" t="s">
-        <v>19</v>
-      </c>
-      <c r="D19">
-        <v>3</v>
-      </c>
-      <c r="E19" s="6">
-        <v>44498</v>
-      </c>
-      <c r="F19" t="s">
+      <c r="B19" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4">
+        <v>3</v>
+      </c>
+      <c r="E19" s="4">
+        <v>3</v>
+      </c>
+      <c r="F19" s="6">
+        <v>44494</v>
+      </c>
+      <c r="G19" s="4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H19" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D20">
         <v>15</v>
       </c>
-      <c r="E20" s="6">
-        <v>44499</v>
-      </c>
-      <c r="F20" t="s">
+      <c r="F20" s="5">
+        <v>44498</v>
+      </c>
+      <c r="G20" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D21">
         <v>5</v>
       </c>
-      <c r="E21" s="6">
-        <v>44500</v>
-      </c>
-      <c r="F21" t="s">
+      <c r="F21" s="5">
+        <v>44499</v>
+      </c>
+      <c r="G21" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>19</v>
       </c>
       <c r="B22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D22">
         <v>5</v>
       </c>
-      <c r="E22" s="6">
-        <v>44501</v>
-      </c>
-      <c r="F22" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F22" s="5">
+        <v>44500</v>
+      </c>
+      <c r="G22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D23">
         <v>10</v>
       </c>
-      <c r="E23" s="6">
-        <v>44502</v>
-      </c>
-      <c r="F23" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F23" s="5">
+        <v>44501</v>
+      </c>
+      <c r="G23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>21</v>
       </c>
       <c r="B24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D24">
         <v>10</v>
       </c>
-      <c r="E24" s="6">
-        <v>44503</v>
+      <c r="F24" s="5">
+        <v>44502</v>
+      </c>
+      <c r="G24" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#10, initial code, comments to be added
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ilja/Code/School/IoT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4751B19F-1B80-5D41-A346-08F778E6AD1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8EE1DD1-2543-7D4D-B2D0-85DF014CB5FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{9D83B715-5ABF-CE44-818A-C1C3B282D9B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
   <si>
     <t>Blinky-blinky</t>
   </si>
@@ -148,6 +148,9 @@
   </si>
   <si>
     <t>Date</t>
+  </si>
+  <si>
+    <t>need to be commented</t>
   </si>
 </sst>
 </file>
@@ -534,7 +537,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -556,7 +559,7 @@
       </c>
       <c r="E1" s="1" t="str">
         <f>_xlfn.CONCAT("Coded ", SUM(E2:E99))</f>
-        <v>Coded 60</v>
+        <v>Coded 75</v>
       </c>
       <c r="F1" t="s">
         <v>37</v>
@@ -924,17 +927,24 @@
       <c r="A20">
         <v>17</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D20">
+      <c r="C20" s="4"/>
+      <c r="D20" s="4">
         <v>15</v>
       </c>
-      <c r="F20" s="5">
-        <v>44498</v>
-      </c>
-      <c r="G20" t="s">
+      <c r="E20" s="4">
+        <v>15</v>
+      </c>
+      <c r="F20" s="6">
+        <v>44495</v>
+      </c>
+      <c r="G20" s="4" t="s">
         <v>30</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
#8 duty cycling 2
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ilja/Code/School/IoT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF2F7B85-7519-4445-849F-A7F55DBDEF1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0DA9993-9D99-CE4B-BD13-A44E028A8403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{9D83B715-5ABF-CE44-818A-C1C3B282D9B7}"/>
   </bookViews>
@@ -229,7 +229,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -250,7 +250,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -267,36 +273,37 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -614,7 +621,7 @@
   <dimension ref="A1:O24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+      <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -661,19 +668,19 @@
       <c r="H1" t="s">
         <v>39</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="6" t="s">
         <v>38</v>
       </c>
       <c r="J1" t="s">
         <v>40</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="6" t="s">
         <v>37</v>
       </c>
       <c r="L1" t="s">
         <v>44</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="M1" s="6" t="s">
         <v>41</v>
       </c>
       <c r="N1" t="s">
@@ -724,25 +731,25 @@
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
-      <c r="H4" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="I4" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="J4" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="K4" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="L4" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="M4" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="N4" s="9" t="s">
+      <c r="H4" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="N4" s="7" t="s">
         <v>42</v>
       </c>
       <c r="O4" s="2"/>
@@ -765,25 +772,25 @@
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
-      <c r="H5" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="I5" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="J5" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="K5" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="L5" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="M5" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="N5" s="9" t="s">
+      <c r="H5" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="N5" s="7" t="s">
         <v>42</v>
       </c>
       <c r="O5" s="2"/>
@@ -806,25 +813,25 @@
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="I6" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="J6" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="K6" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="L6" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="M6" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="N6" s="9" t="s">
+      <c r="H6" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="L6" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="N6" s="7" t="s">
         <v>42</v>
       </c>
       <c r="O6" s="2"/>
@@ -847,25 +854,25 @@
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="I7" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="J7" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="K7" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="L7" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="M7" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="N7" s="9" t="s">
+      <c r="H7" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="L7" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="M7" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="N7" s="7" t="s">
         <v>42</v>
       </c>
       <c r="O7" s="2"/>
@@ -888,25 +895,25 @@
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
-      <c r="H8" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="I8" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="J8" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="K8" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="L8" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="M8" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="N8" s="9" t="s">
+      <c r="H8" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="L8" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="M8" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="N8" s="7" t="s">
         <v>42</v>
       </c>
       <c r="O8" s="2"/>
@@ -929,25 +936,25 @@
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
-      <c r="H9" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="I9" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="J9" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="K9" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="L9" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="M9" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="N9" s="9" t="s">
+      <c r="H9" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="L9" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="M9" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="N9" s="7" t="s">
         <v>42</v>
       </c>
       <c r="O9" s="2"/>
@@ -970,25 +977,25 @@
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
-      <c r="H10" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="I10" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="J10" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="K10" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="L10" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="M10" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="N10" s="9" t="s">
+      <c r="H10" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="L10" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="M10" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="N10" s="7" t="s">
         <v>42</v>
       </c>
       <c r="O10" s="2"/>
@@ -1011,25 +1018,25 @@
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
-      <c r="H11" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="I11" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="J11" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="K11" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="L11" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="M11" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="N11" s="9" t="s">
+      <c r="H11" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="K11" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="L11" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="M11" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="N11" s="7" t="s">
         <v>42</v>
       </c>
       <c r="O11" s="2"/>
@@ -1054,25 +1061,25 @@
       <c r="G12" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="H12" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="I12" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="J12" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="K12" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="L12" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="M12" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="N12" s="9" t="s">
+      <c r="H12" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="J12" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="K12" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="L12" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="M12" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="N12" s="7" t="s">
         <v>42</v>
       </c>
       <c r="O12" s="2"/>
@@ -1081,132 +1088,132 @@
       <c r="A13">
         <v>10</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="15">
+      <c r="C13" s="9">
         <v>4</v>
       </c>
-      <c r="D13" s="15">
+      <c r="D13" s="9">
         <v>4</v>
       </c>
-      <c r="E13" s="15">
+      <c r="E13" s="9">
         <v>4</v>
       </c>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15" t="s">
+      <c r="F13" s="9"/>
+      <c r="G13" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="H13" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="I13" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="J13" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="K13" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="L13" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="M13" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="N13" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="O13" s="15"/>
+      <c r="H13" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="J13" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="K13" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="L13" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="M13" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="N13" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="O13" s="9"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>11</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="15">
+      <c r="C14" s="9">
         <v>4</v>
       </c>
-      <c r="D14" s="15">
+      <c r="D14" s="9">
         <v>4</v>
       </c>
-      <c r="E14" s="15">
+      <c r="E14" s="9">
         <v>4</v>
       </c>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15" t="s">
+      <c r="F14" s="9"/>
+      <c r="G14" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="H14" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="I14" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="J14" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="K14" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="L14" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="M14" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="N14" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="O14" s="15"/>
+      <c r="H14" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="J14" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="K14" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="L14" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="M14" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="N14" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="O14" s="9"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>12</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="15">
-        <v>3</v>
-      </c>
-      <c r="D15" s="15">
-        <v>3</v>
-      </c>
-      <c r="E15" s="15">
-        <v>3</v>
-      </c>
-      <c r="F15" s="17">
+      <c r="C15" s="9">
+        <v>3</v>
+      </c>
+      <c r="D15" s="9">
+        <v>3</v>
+      </c>
+      <c r="E15" s="9">
+        <v>3</v>
+      </c>
+      <c r="F15" s="11">
         <v>44494</v>
       </c>
-      <c r="G15" s="15" t="s">
+      <c r="G15" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="H15" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="I15" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="J15" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="K15" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="L15" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="M15" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="N15" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="O15" s="15"/>
+      <c r="H15" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="J15" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="K15" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="L15" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="M15" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="N15" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="O15" s="9"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16">
@@ -1230,28 +1237,28 @@
       <c r="G16" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="H16" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="I16" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="J16" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="K16" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="L16" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="M16" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="N16" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="O16" s="11" t="s">
+      <c r="H16" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="I16" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="J16" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="K16" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="L16" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="M16" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="N16" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="O16" s="16" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1277,28 +1284,28 @@
       <c r="G17" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="H17" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="I17" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="J17" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="K17" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="L17" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="M17" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="N17" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="O17" s="11" t="s">
+      <c r="H17" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="I17" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="J17" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="K17" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="L17" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="M17" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="N17" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="O17" s="16" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1316,25 +1323,25 @@
       <c r="E18" s="3">
         <v>4</v>
       </c>
-      <c r="F18" s="5">
+      <c r="F18" s="4">
         <v>44500</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="H18" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="I18" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10" t="s">
+      <c r="H18" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="L18" s="10"/>
-      <c r="M18" s="10"/>
-      <c r="N18" s="10"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="8"/>
       <c r="O18" s="3"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
@@ -1353,34 +1360,34 @@
       <c r="E19" s="2">
         <v>3</v>
       </c>
-      <c r="F19" s="18">
+      <c r="F19" s="12">
         <v>44494</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H19" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="I19" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="J19" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="K19" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="L19" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="M19" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="N19" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="O19" s="15"/>
+      <c r="H19" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I19" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="J19" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="K19" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="L19" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="M19" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="N19" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="O19" s="9"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20">
@@ -1396,23 +1403,23 @@
       <c r="E20" s="3">
         <v>15</v>
       </c>
-      <c r="F20" s="5">
+      <c r="F20" s="4">
         <v>44495</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H20" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="I20" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="J20" s="10"/>
-      <c r="K20" s="10"/>
-      <c r="L20" s="10"/>
-      <c r="M20" s="10"/>
-      <c r="N20" s="10"/>
+      <c r="H20" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="I20" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="J20" s="8"/>
+      <c r="K20" s="8"/>
+      <c r="L20" s="8"/>
+      <c r="M20" s="8"/>
+      <c r="N20" s="8"/>
       <c r="O20" s="3" t="s">
         <v>35</v>
       </c>
@@ -1431,25 +1438,25 @@
       <c r="E21" s="3">
         <v>5</v>
       </c>
-      <c r="F21" s="5">
+      <c r="F21" s="4">
         <v>44503</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="H21" s="10"/>
-      <c r="I21" s="10"/>
-      <c r="J21" s="10"/>
-      <c r="K21" s="10"/>
-      <c r="L21" s="10"/>
-      <c r="M21" s="10"/>
-      <c r="N21" s="10"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="8"/>
+      <c r="M21" s="8"/>
+      <c r="N21" s="8"/>
       <c r="O21" s="3" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A22" s="6">
+      <c r="A22" s="5">
         <v>19</v>
       </c>
       <c r="B22" s="3" t="s">
@@ -1462,23 +1469,23 @@
       <c r="E22" s="3">
         <v>5</v>
       </c>
-      <c r="F22" s="5">
+      <c r="F22" s="4">
         <v>44496</v>
       </c>
       <c r="G22" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="H22" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="I22" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="J22" s="10"/>
-      <c r="K22" s="10"/>
-      <c r="L22" s="10"/>
-      <c r="M22" s="10"/>
-      <c r="N22" s="10"/>
+      <c r="H22" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="I22" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="8"/>
+      <c r="M22" s="8"/>
+      <c r="N22" s="8"/>
       <c r="O22" s="3" t="s">
         <v>35</v>
       </c>
@@ -1497,23 +1504,23 @@
       <c r="E23" s="3">
         <v>10</v>
       </c>
-      <c r="F23" s="5">
+      <c r="F23" s="4">
         <v>44501</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="H23" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="I23" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="J23" s="10"/>
-      <c r="K23" s="10"/>
-      <c r="L23" s="10"/>
-      <c r="M23" s="10"/>
-      <c r="N23" s="10"/>
+      <c r="H23" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="I23" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="8"/>
+      <c r="M23" s="8"/>
+      <c r="N23" s="8"/>
       <c r="O23" s="3" t="s">
         <v>51</v>
       </c>
@@ -1522,28 +1529,30 @@
       <c r="A24">
         <v>21</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="D24">
+      <c r="C24" s="17"/>
+      <c r="D24" s="17">
         <v>10</v>
       </c>
-      <c r="F24" s="4">
+      <c r="E24" s="17"/>
+      <c r="F24" s="18">
         <v>44502</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G24" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="H24" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="I24" s="8"/>
-      <c r="J24" s="8"/>
-      <c r="K24" s="8"/>
-      <c r="L24" s="8"/>
-      <c r="M24" s="8"/>
-      <c r="N24" s="8"/>
-      <c r="O24" s="3" t="s">
+      <c r="H24" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="I24" s="19"/>
+      <c r="J24" s="19"/>
+      <c r="K24" s="19"/>
+      <c r="L24" s="19"/>
+      <c r="M24" s="19"/>
+      <c r="N24" s="19"/>
+      <c r="O24" s="17" t="s">
         <v>52</v>
       </c>
     </row>

</xml_diff>

<commit_message>
#8, final version, commented code, scheme
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ilja/Code/School/IoT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B88A3495-74D6-FA46-9D5B-CDA74087234A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D4A120C-78F0-584E-AB3E-750D8C0150F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{9D83B715-5ABF-CE44-818A-C1C3B282D9B7}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="52">
   <si>
     <t>Blinky-blinky</t>
   </si>
@@ -180,7 +180,7 @@
     <t>#2</t>
   </si>
   <si>
-    <t>ok?</t>
+    <t>Waiting for JACF</t>
   </si>
   <si>
     <t>ESP32 code done</t>
@@ -226,7 +226,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -242,6 +242,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -264,7 +270,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -287,6 +293,11 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -606,7 +617,7 @@
   <dimension ref="A1:O24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -634,7 +645,7 @@
       <c r="B1" s="1"/>
       <c r="C1" s="1" t="str">
         <f>_xlfn.CONCAT("Current ", SUM(C2:C99))</f>
-        <v>Current 56</v>
+        <v>Current 57</v>
       </c>
       <c r="D1" s="1" t="str">
         <f>_xlfn.CONCAT("Max ", SUM(D2:D99))</f>
@@ -642,7 +653,7 @@
       </c>
       <c r="E1" s="1" t="str">
         <f>_xlfn.CONCAT("Coded ", SUM(E2:E99))</f>
-        <v>Coded 95</v>
+        <v>Coded 100</v>
       </c>
       <c r="F1" t="s">
         <v>34</v>
@@ -1294,38 +1305,48 @@
       <c r="A18">
         <v>15</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3">
+      <c r="C18" s="13">
+        <v>1</v>
+      </c>
+      <c r="D18" s="13">
         <v>4</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E18" s="13">
         <v>4</v>
       </c>
-      <c r="F18" s="4">
+      <c r="F18" s="14">
         <v>44500</v>
       </c>
-      <c r="G18" s="3" t="s">
+      <c r="G18" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="H18" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="I18" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="J18" s="8"/>
-      <c r="K18" s="8" t="s">
+      <c r="H18" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="I18" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="J18" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="K18" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="L18" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="M18" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="N18" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="O18" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="L18" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="M18" s="8"/>
-      <c r="N18" s="8"/>
-      <c r="O18" s="3"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19">
@@ -1427,8 +1448,12 @@
       <c r="G21" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
+      <c r="H21" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="I21" s="8" t="s">
+        <v>42</v>
+      </c>
       <c r="J21" s="8"/>
       <c r="K21" s="8"/>
       <c r="L21" s="8"/>
@@ -1512,30 +1537,32 @@
       <c r="A24">
         <v>21</v>
       </c>
-      <c r="B24" s="13" t="s">
+      <c r="B24" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13">
+      <c r="C24" s="16"/>
+      <c r="D24" s="16">
         <v>10</v>
       </c>
-      <c r="E24" s="13"/>
-      <c r="F24" s="14">
+      <c r="E24" s="16">
+        <v>5</v>
+      </c>
+      <c r="F24" s="17">
         <v>44502</v>
       </c>
-      <c r="G24" s="13" t="s">
+      <c r="G24" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="H24" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="I24" s="15"/>
-      <c r="J24" s="15"/>
-      <c r="K24" s="15"/>
-      <c r="L24" s="15"/>
-      <c r="M24" s="15"/>
-      <c r="N24" s="15"/>
-      <c r="O24" s="13" t="s">
+      <c r="H24" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="I24" s="18"/>
+      <c r="J24" s="18"/>
+      <c r="K24" s="18"/>
+      <c r="L24" s="18"/>
+      <c r="M24" s="18"/>
+      <c r="N24" s="18"/>
+      <c r="O24" s="16" t="s">
         <v>51</v>
       </c>
     </row>

</xml_diff>

<commit_message>
#14 1Wire like communication
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ilja/Code/School/IoT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D4A120C-78F0-584E-AB3E-750D8C0150F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B95F256-CE3F-EB45-B269-24B88670D872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{9D83B715-5ABF-CE44-818A-C1C3B282D9B7}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="51">
   <si>
     <t>Blinky-blinky</t>
   </si>
@@ -178,9 +178,6 @@
   </si>
   <si>
     <t>#2</t>
-  </si>
-  <si>
-    <t>Waiting for JACF</t>
   </si>
   <si>
     <t>ESP32 code done</t>
@@ -226,7 +223,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -242,12 +239,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -270,7 +261,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -293,11 +284,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -617,7 +603,7 @@
   <dimension ref="A1:O24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -645,7 +631,7 @@
       <c r="B1" s="1"/>
       <c r="C1" s="1" t="str">
         <f>_xlfn.CONCAT("Current ", SUM(C2:C99))</f>
-        <v>Current 57</v>
+        <v>Current 60</v>
       </c>
       <c r="D1" s="1" t="str">
         <f>_xlfn.CONCAT("Max ", SUM(D2:D99))</f>
@@ -1305,48 +1291,46 @@
       <c r="A18">
         <v>15</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="13">
-        <v>1</v>
-      </c>
-      <c r="D18" s="13">
-        <v>4</v>
-      </c>
-      <c r="E18" s="13">
-        <v>4</v>
-      </c>
-      <c r="F18" s="14">
+      <c r="C18" s="2">
+        <v>4</v>
+      </c>
+      <c r="D18" s="2">
+        <v>4</v>
+      </c>
+      <c r="E18" s="2">
+        <v>4</v>
+      </c>
+      <c r="F18" s="12">
         <v>44500</v>
       </c>
-      <c r="G18" s="13" t="s">
+      <c r="G18" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="H18" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="I18" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="J18" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="K18" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="L18" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="M18" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="N18" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="O18" s="13" t="s">
-        <v>48</v>
-      </c>
+      <c r="H18" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I18" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="J18" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="K18" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="L18" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="M18" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="N18" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="O18" s="2"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19">
@@ -1460,7 +1444,7 @@
       <c r="M21" s="8"/>
       <c r="N21" s="8"/>
       <c r="O21" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
@@ -1530,40 +1514,40 @@
       <c r="M23" s="8"/>
       <c r="N23" s="8"/>
       <c r="O23" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>21</v>
       </c>
-      <c r="B24" s="16" t="s">
+      <c r="B24" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="16"/>
-      <c r="D24" s="16">
+      <c r="C24" s="13"/>
+      <c r="D24" s="13">
         <v>10</v>
       </c>
-      <c r="E24" s="16">
+      <c r="E24" s="13">
         <v>5</v>
       </c>
-      <c r="F24" s="17">
+      <c r="F24" s="14">
         <v>44502</v>
       </c>
-      <c r="G24" s="16" t="s">
+      <c r="G24" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="H24" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="I24" s="18"/>
-      <c r="J24" s="18"/>
-      <c r="K24" s="18"/>
-      <c r="L24" s="18"/>
-      <c r="M24" s="18"/>
-      <c r="N24" s="18"/>
-      <c r="O24" s="16" t="s">
-        <v>51</v>
+      <c r="H24" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="I24" s="15"/>
+      <c r="J24" s="15"/>
+      <c r="K24" s="15"/>
+      <c r="L24" s="15"/>
+      <c r="M24" s="15"/>
+      <c r="N24" s="15"/>
+      <c r="O24" s="13" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#12, misquittoes final touch
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ilja/Code/School/IoT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B95F256-CE3F-EB45-B269-24B88670D872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F34E4685-FE69-BD40-A7ED-B17011AA100C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{9D83B715-5ABF-CE44-818A-C1C3B282D9B7}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="51">
   <si>
     <t>Blinky-blinky</t>
   </si>
@@ -141,9 +141,6 @@
     <t>Date</t>
   </si>
   <si>
-    <t>need to be commented</t>
-  </si>
-  <si>
     <t>#</t>
   </si>
   <si>
@@ -180,13 +177,16 @@
     <t>#2</t>
   </si>
   <si>
-    <t>ESP32 code done</t>
-  </si>
-  <si>
     <t>can be upgraded, comments needed</t>
   </si>
   <si>
     <t>code in process</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Submitted, waiting for JACF</t>
   </si>
 </sst>
 </file>
@@ -223,7 +223,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -248,6 +248,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -261,7 +267,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -284,6 +290,11 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -603,7 +614,7 @@
   <dimension ref="A1:O24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="O23" sqref="O23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -612,7 +623,7 @@
     <col min="2" max="2" width="34.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="4.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="5" bestFit="1" customWidth="1"/>
@@ -626,12 +637,12 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1" t="str">
         <f>_xlfn.CONCAT("Current ", SUM(C2:C99))</f>
-        <v>Current 60</v>
+        <v>Current 80</v>
       </c>
       <c r="D1" s="1" t="str">
         <f>_xlfn.CONCAT("Max ", SUM(D2:D99))</f>
@@ -648,25 +659,25 @@
         <v>24</v>
       </c>
       <c r="H1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="J1" t="s">
         <v>39</v>
       </c>
-      <c r="I1" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="K1" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="L1" t="s">
+        <v>43</v>
+      </c>
+      <c r="M1" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="K1" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="L1" t="s">
-        <v>44</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>41</v>
-      </c>
       <c r="N1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
@@ -714,25 +725,25 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L4" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N4" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O4" s="2"/>
     </row>
@@ -755,25 +766,25 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L5" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N5" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O5" s="2"/>
     </row>
@@ -796,25 +807,25 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L6" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N6" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O6" s="2"/>
     </row>
@@ -837,25 +848,25 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K7" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L7" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M7" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N7" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O7" s="2"/>
     </row>
@@ -878,25 +889,25 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K8" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L8" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M8" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N8" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O8" s="2"/>
     </row>
@@ -919,25 +930,25 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K9" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L9" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M9" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N9" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O9" s="2"/>
     </row>
@@ -960,25 +971,25 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K10" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L10" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M10" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N10" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O10" s="2"/>
     </row>
@@ -1001,25 +1012,25 @@
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K11" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L11" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M11" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N11" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O11" s="2"/>
     </row>
@@ -1041,28 +1052,28 @@
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K12" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L12" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M12" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N12" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O12" s="2"/>
     </row>
@@ -1084,28 +1095,28 @@
       </c>
       <c r="F13" s="9"/>
       <c r="G13" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J13" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K13" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L13" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M13" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N13" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O13" s="9"/>
     </row>
@@ -1127,28 +1138,28 @@
       </c>
       <c r="F14" s="9"/>
       <c r="G14" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K14" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L14" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M14" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N14" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O14" s="9"/>
     </row>
@@ -1175,25 +1186,25 @@
         <v>25</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K15" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L15" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M15" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N15" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O15" s="9"/>
     </row>
@@ -1220,25 +1231,25 @@
         <v>23</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K16" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L16" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M16" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N16" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O16" s="9"/>
     </row>
@@ -1265,25 +1276,25 @@
         <v>26</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K17" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L17" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M17" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N17" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O17" s="9"/>
     </row>
@@ -1310,25 +1321,25 @@
         <v>27</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K18" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L18" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M18" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N18" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O18" s="2"/>
     </row>
@@ -1355,25 +1366,25 @@
         <v>28</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K19" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L19" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M19" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N19" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O19" s="9"/>
     </row>
@@ -1381,105 +1392,135 @@
       <c r="A20">
         <v>17</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3">
+      <c r="C20" s="2">
         <v>15</v>
       </c>
-      <c r="E20" s="3">
+      <c r="D20" s="2">
         <v>15</v>
       </c>
-      <c r="F20" s="4">
+      <c r="E20" s="2">
+        <v>15</v>
+      </c>
+      <c r="F20" s="12">
         <v>44495</v>
       </c>
-      <c r="G20" s="3" t="s">
+      <c r="G20" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H20" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="I20" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="J20" s="8"/>
-      <c r="K20" s="8"/>
-      <c r="L20" s="8"/>
-      <c r="M20" s="8"/>
-      <c r="N20" s="8"/>
-      <c r="O20" s="3" t="s">
-        <v>35</v>
-      </c>
+      <c r="H20" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="J20" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="K20" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="L20" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="M20" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="N20" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="O20" s="2"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>18</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3">
+      <c r="C21" s="2">
         <v>5</v>
       </c>
-      <c r="E21" s="3">
+      <c r="D21" s="2">
         <v>5</v>
       </c>
-      <c r="F21" s="4">
+      <c r="E21" s="2">
+        <v>5</v>
+      </c>
+      <c r="F21" s="12">
         <v>44503</v>
       </c>
-      <c r="G21" s="3" t="s">
+      <c r="G21" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H21" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="I21" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="J21" s="8"/>
-      <c r="K21" s="8"/>
-      <c r="L21" s="8"/>
-      <c r="M21" s="8"/>
-      <c r="N21" s="8"/>
-      <c r="O21" s="3" t="s">
-        <v>48</v>
-      </c>
+      <c r="H21" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="I21" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="J21" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="K21" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="L21" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="M21" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="N21" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="O21" s="2"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" s="5">
         <v>19</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3">
+      <c r="C22" s="16"/>
+      <c r="D22" s="16">
         <v>5</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E22" s="16">
         <v>5</v>
       </c>
-      <c r="F22" s="4">
+      <c r="F22" s="17">
         <v>44496</v>
       </c>
-      <c r="G22" s="3" t="s">
+      <c r="G22" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="H22" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="I22" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="J22" s="8"/>
-      <c r="K22" s="8"/>
-      <c r="L22" s="8"/>
-      <c r="M22" s="8"/>
-      <c r="N22" s="8"/>
-      <c r="O22" s="3" t="s">
-        <v>35</v>
+      <c r="H22" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="I22" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="J22" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="K22" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="L22" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="M22" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="N22" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="O22" s="16" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
@@ -1503,10 +1544,10 @@
         <v>32</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I23" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J23" s="8"/>
       <c r="K23" s="8"/>
@@ -1514,7 +1555,7 @@
       <c r="M23" s="8"/>
       <c r="N23" s="8"/>
       <c r="O23" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
@@ -1538,7 +1579,7 @@
         <v>33</v>
       </c>
       <c r="H24" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I24" s="15"/>
       <c r="J24" s="15"/>
@@ -1547,7 +1588,7 @@
       <c r="M24" s="15"/>
       <c r="N24" s="15"/>
       <c r="O24" s="13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>